<commit_message>
Refactorizado el codigo y creado diagrama de flujo
</commit_message>
<xml_diff>
--- a/AppVehiculos/resources/SistemasVehiculos.xlsx
+++ b/AppVehiculos/resources/SistemasVehiculos.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="848">
   <si>
     <t>Nombre</t>
   </si>
@@ -1975,6 +1975,114 @@
     <t>25187786001225455548</t>
   </si>
   <si>
+    <t>09763856B</t>
+  </si>
+  <si>
+    <t>09768995K</t>
+  </si>
+  <si>
+    <t>09770039F</t>
+  </si>
+  <si>
+    <t>09774163Z</t>
+  </si>
+  <si>
+    <t>09774199G</t>
+  </si>
+  <si>
+    <t>09798076F</t>
+  </si>
+  <si>
+    <t>09798287B</t>
+  </si>
+  <si>
+    <t>09799247M</t>
+  </si>
+  <si>
+    <t>09800420M</t>
+  </si>
+  <si>
+    <t>09800921T</t>
+  </si>
+  <si>
+    <t>09801107W</t>
+  </si>
+  <si>
+    <t>11437269J</t>
+  </si>
+  <si>
+    <t>11637421L</t>
+  </si>
+  <si>
+    <t>11966672W</t>
+  </si>
+  <si>
+    <t>11662128R</t>
+  </si>
+  <si>
+    <t>11673213T</t>
+  </si>
+  <si>
+    <t>11942643P</t>
+  </si>
+  <si>
+    <t>11971207Y</t>
+  </si>
+  <si>
+    <t>11957847D</t>
+  </si>
+  <si>
+    <t>11959249P</t>
+  </si>
+  <si>
+    <t>11959694Q</t>
+  </si>
+  <si>
+    <t>00750184330702510011</t>
+  </si>
+  <si>
+    <t>21508149175421346497</t>
+  </si>
+  <si>
+    <t>21346154503164978451</t>
+  </si>
+  <si>
+    <t>25187786311225455548</t>
+  </si>
+  <si>
+    <t>63516541828944000984</t>
+  </si>
+  <si>
+    <t>23658965274585223202</t>
+  </si>
+  <si>
+    <t>32658012367712548745</t>
+  </si>
+  <si>
+    <t>23652365142254222000</t>
+  </si>
+  <si>
+    <t>20012541150023365233</t>
+  </si>
+  <si>
+    <t>32584216971684051000</t>
+  </si>
+  <si>
+    <t>65645150865168448896</t>
+  </si>
+  <si>
+    <t>26551681807651415636</t>
+  </si>
+  <si>
+    <t>99558741836555551120</t>
+  </si>
+  <si>
+    <t>52198484752100515144</t>
+  </si>
+  <si>
+    <t>51556584221251000254</t>
+  </si>
+  <si>
     <t>GR9420125003305201112544</t>
   </si>
   <si>
@@ -2005,9 +2113,6 @@
     <t>ACP00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>00750184330702510011</t>
-  </si>
-  <si>
     <t>SM5925894363435485700142</t>
   </si>
   <si>
@@ -2104,15 +2209,6 @@
     <t>GMM02@vehiculos2025.com</t>
   </si>
   <si>
-    <t>21508149175421346497</t>
-  </si>
-  <si>
-    <t>21346154503164978451</t>
-  </si>
-  <si>
-    <t>25187786311225455548</t>
-  </si>
-  <si>
     <t>ES4723164897642213030615</t>
   </si>
   <si>
@@ -2185,21 +2281,6 @@
     <t>IAG00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09763856B</t>
-  </si>
-  <si>
-    <t>09768995K</t>
-  </si>
-  <si>
-    <t>09770039F</t>
-  </si>
-  <si>
-    <t>09774163Z</t>
-  </si>
-  <si>
-    <t>09774199G</t>
-  </si>
-  <si>
     <t>ES8020960043033000100000</t>
   </si>
   <si>
@@ -2305,72 +2386,36 @@
     <t>FDL00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09798076F</t>
-  </si>
-  <si>
-    <t>63516541828944000984</t>
-  </si>
-  <si>
     <t>ES8163516541828944000984</t>
   </si>
   <si>
     <t>SDM00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09798287B</t>
-  </si>
-  <si>
-    <t>23658965274585223202</t>
-  </si>
-  <si>
     <t>ES6223658965274585223202</t>
   </si>
   <si>
     <t>EGM00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09799247M</t>
-  </si>
-  <si>
-    <t>32658012367712548745</t>
-  </si>
-  <si>
     <t>FI6132658012367712548745</t>
   </si>
   <si>
     <t>GPM00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09800420M</t>
-  </si>
-  <si>
-    <t>23652365142254222000</t>
-  </si>
-  <si>
     <t>ES7223652365142254222000</t>
   </si>
   <si>
     <t>EAM00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09800921T</t>
-  </si>
-  <si>
-    <t>20012541150023365233</t>
-  </si>
-  <si>
     <t>FR3820012541150023365233</t>
   </si>
   <si>
     <t>MMM00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>09801107W</t>
-  </si>
-  <si>
-    <t>32584216971684051000</t>
-  </si>
-  <si>
     <t>ES9232584216971684051000</t>
   </si>
   <si>
@@ -2437,133 +2482,88 @@
     <t>KSC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>65645150865168448896</t>
-  </si>
-  <si>
     <t>AT8365645150865168448896</t>
   </si>
   <si>
     <t>MHC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>26551681807651415636</t>
-  </si>
-  <si>
     <t>IT3526551681807651415636</t>
   </si>
   <si>
     <t>CLD00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>99558741836555551120</t>
-  </si>
-  <si>
     <t>HU2399558741836555551120</t>
   </si>
   <si>
     <t>MFD00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>52198484752100515144</t>
-  </si>
-  <si>
     <t>ES4352198484752100515144</t>
   </si>
   <si>
     <t>FGD00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>51556584221251000254</t>
-  </si>
-  <si>
     <t>IE6851556584221251000254</t>
   </si>
   <si>
     <t>GMM04@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11437269J</t>
-  </si>
-  <si>
     <t>DK9632541112811220000577</t>
   </si>
   <si>
     <t>IVC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11637421L</t>
-  </si>
-  <si>
     <t>LT9362541122421110105611</t>
   </si>
   <si>
     <t>DMC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11966672W</t>
-  </si>
-  <si>
     <t>ES6855065688761051056105</t>
   </si>
   <si>
     <t>EBC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11662128R</t>
-  </si>
-  <si>
     <t>ES7426221011628048788896</t>
   </si>
   <si>
     <t>NBC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11673213T</t>
-  </si>
-  <si>
     <t>ES9712548521518742146695</t>
   </si>
   <si>
     <t>MSC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11942643P</t>
-  </si>
-  <si>
     <t>ES9001826530120201560000</t>
   </si>
   <si>
     <t>MDC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11971207Y</t>
-  </si>
-  <si>
     <t>ES0421651651812511133547</t>
   </si>
   <si>
     <t>MFC00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11957847D</t>
-  </si>
-  <si>
     <t>ES6851651487910005118185</t>
   </si>
   <si>
     <t>CDD00@vehiculos2025.com</t>
   </si>
   <si>
-    <t>11959249P</t>
-  </si>
-  <si>
     <t>CZ9536250012804785523365</t>
   </si>
   <si>
     <t>CGD00@vehiculos2025.com</t>
-  </si>
-  <si>
-    <t>11959694Q</t>
   </si>
   <si>
     <t>AT2522515651915640081011</t>
@@ -3210,7 +3210,7 @@
         <v>277</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>650</v>
+        <v>686</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>509</v>
@@ -3222,7 +3222,7 @@
         <v>144</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>649</v>
+        <v>685</v>
       </c>
       <c r="L8" s="0">
         <v>0</v>
@@ -3248,7 +3248,7 @@
         <v>277</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>652</v>
+        <v>688</v>
       </c>
       <c r="H9" t="s" s="0">
         <v>509</v>
@@ -3260,7 +3260,7 @@
         <v>145</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>651</v>
+        <v>687</v>
       </c>
       <c r="L9" s="0">
         <v>0</v>
@@ -3286,7 +3286,7 @@
         <v>278</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>654</v>
+        <v>690</v>
       </c>
       <c r="H10" t="s" s="0">
         <v>509</v>
@@ -3298,7 +3298,7 @@
         <v>146</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>653</v>
+        <v>689</v>
       </c>
       <c r="L10" s="0">
         <v>0</v>
@@ -3324,7 +3324,7 @@
         <v>279</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>656</v>
+        <v>692</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>509</v>
@@ -3336,7 +3336,7 @@
         <v>147</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>655</v>
+        <v>691</v>
       </c>
       <c r="L11" s="0">
         <v>0</v>
@@ -3362,7 +3362,7 @@
         <v>279</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>658</v>
+        <v>694</v>
       </c>
       <c r="H12" t="s" s="0">
         <v>509</v>
@@ -3374,7 +3374,7 @@
         <v>148</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>657</v>
+        <v>693</v>
       </c>
       <c r="L12" s="0">
         <v>0</v>
@@ -3436,7 +3436,7 @@
         <v>216</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>659</v>
+        <v>670</v>
       </c>
       <c r="L14" s="0">
         <v>0</v>
@@ -3468,7 +3468,7 @@
         <v>282</v>
       </c>
       <c r="G16" t="s" s="0">
-        <v>661</v>
+        <v>696</v>
       </c>
       <c r="H16" t="s" s="0">
         <v>509</v>
@@ -3480,7 +3480,7 @@
         <v>599</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>660</v>
+        <v>695</v>
       </c>
       <c r="L16" s="0">
         <v>0</v>
@@ -3506,7 +3506,7 @@
         <v>283</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>663</v>
+        <v>698</v>
       </c>
       <c r="H17" t="s" s="0">
         <v>509</v>
@@ -3518,7 +3518,7 @@
         <v>600</v>
       </c>
       <c r="K17" t="s" s="0">
-        <v>662</v>
+        <v>697</v>
       </c>
       <c r="L17" s="0">
         <v>0</v>
@@ -3544,7 +3544,7 @@
         <v>283</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>665</v>
+        <v>700</v>
       </c>
       <c r="H18" t="s" s="0">
         <v>509</v>
@@ -3556,7 +3556,7 @@
         <v>151</v>
       </c>
       <c r="K18" t="s" s="0">
-        <v>664</v>
+        <v>699</v>
       </c>
       <c r="L18" s="0">
         <v>0</v>
@@ -3582,7 +3582,7 @@
         <v>282</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>667</v>
+        <v>702</v>
       </c>
       <c r="H19" t="s" s="0">
         <v>509</v>
@@ -3594,7 +3594,7 @@
         <v>152</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>666</v>
+        <v>701</v>
       </c>
       <c r="L19" s="0">
         <v>0</v>
@@ -3620,7 +3620,7 @@
         <v>282</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>669</v>
+        <v>704</v>
       </c>
       <c r="H20" t="s" s="0">
         <v>509</v>
@@ -3632,7 +3632,7 @@
         <v>153</v>
       </c>
       <c r="K20" t="s" s="0">
-        <v>668</v>
+        <v>703</v>
       </c>
       <c r="L20" s="0">
         <v>0</v>
@@ -3658,7 +3658,7 @@
         <v>283</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>671</v>
+        <v>706</v>
       </c>
       <c r="H21" t="s" s="0">
         <v>509</v>
@@ -3670,7 +3670,7 @@
         <v>150</v>
       </c>
       <c r="K21" t="s" s="0">
-        <v>670</v>
+        <v>705</v>
       </c>
       <c r="L21" s="0">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>284</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>673</v>
+        <v>708</v>
       </c>
       <c r="H22" t="s" s="0">
         <v>509</v>
@@ -3708,7 +3708,7 @@
         <v>154</v>
       </c>
       <c r="K22" t="s" s="0">
-        <v>672</v>
+        <v>707</v>
       </c>
       <c r="L22" s="0">
         <v>0</v>
@@ -3734,7 +3734,7 @@
         <v>285</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>675</v>
+        <v>710</v>
       </c>
       <c r="H23" t="s" s="0">
         <v>509</v>
@@ -3746,7 +3746,7 @@
         <v>155</v>
       </c>
       <c r="K23" t="s" s="0">
-        <v>674</v>
+        <v>709</v>
       </c>
       <c r="L23" s="0">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>283</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>677</v>
+        <v>712</v>
       </c>
       <c r="H24" t="s" s="0">
         <v>509</v>
@@ -3784,7 +3784,7 @@
         <v>156</v>
       </c>
       <c r="K24" t="s" s="0">
-        <v>676</v>
+        <v>711</v>
       </c>
       <c r="L24" s="0">
         <v>0</v>
@@ -3810,7 +3810,7 @@
         <v>286</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>679</v>
+        <v>714</v>
       </c>
       <c r="H25" t="s" s="0">
         <v>509</v>
@@ -3822,7 +3822,7 @@
         <v>157</v>
       </c>
       <c r="K25" t="s" s="0">
-        <v>678</v>
+        <v>713</v>
       </c>
       <c r="L25" s="0">
         <v>0</v>
@@ -3854,7 +3854,7 @@
         <v>283</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>681</v>
+        <v>716</v>
       </c>
       <c r="H27" t="s" s="0">
         <v>509</v>
@@ -3866,7 +3866,7 @@
         <v>158</v>
       </c>
       <c r="K27" t="s" s="0">
-        <v>680</v>
+        <v>715</v>
       </c>
       <c r="L27" s="0">
         <v>0</v>
@@ -3892,7 +3892,7 @@
         <v>276</v>
       </c>
       <c r="G28" t="s" s="0">
-        <v>683</v>
+        <v>718</v>
       </c>
       <c r="H28" t="s" s="0">
         <v>509</v>
@@ -3904,7 +3904,7 @@
         <v>159</v>
       </c>
       <c r="K28" t="s" s="0">
-        <v>682</v>
+        <v>717</v>
       </c>
       <c r="L28" s="0">
         <v>0</v>
@@ -3930,7 +3930,7 @@
         <v>280</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>685</v>
+        <v>720</v>
       </c>
       <c r="H29" t="s" s="0">
         <v>509</v>
@@ -3942,7 +3942,7 @@
         <v>160</v>
       </c>
       <c r="K29" t="s" s="0">
-        <v>684</v>
+        <v>719</v>
       </c>
       <c r="L29" s="0">
         <v>0</v>
@@ -3968,7 +3968,7 @@
         <v>280</v>
       </c>
       <c r="G30" t="s" s="0">
-        <v>687</v>
+        <v>722</v>
       </c>
       <c r="H30" t="s" s="0">
         <v>509</v>
@@ -3980,7 +3980,7 @@
         <v>161</v>
       </c>
       <c r="K30" t="s" s="0">
-        <v>686</v>
+        <v>721</v>
       </c>
       <c r="L30" s="0">
         <v>0</v>
@@ -4006,7 +4006,7 @@
         <v>280</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>689</v>
+        <v>724</v>
       </c>
       <c r="H31" t="s" s="0">
         <v>509</v>
@@ -4018,7 +4018,7 @@
         <v>162</v>
       </c>
       <c r="K31" t="s" s="0">
-        <v>688</v>
+        <v>723</v>
       </c>
       <c r="L31" s="0">
         <v>0</v>
@@ -4044,7 +4044,7 @@
         <v>287</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>691</v>
+        <v>726</v>
       </c>
       <c r="H32" t="s" s="0">
         <v>509</v>
@@ -4056,7 +4056,7 @@
         <v>163</v>
       </c>
       <c r="K32" t="s" s="0">
-        <v>690</v>
+        <v>725</v>
       </c>
       <c r="L32" s="0">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>210</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>692</v>
+        <v>671</v>
       </c>
       <c r="L36" s="0">
         <v>0</v>
@@ -4138,7 +4138,7 @@
         <v>210</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>693</v>
+        <v>672</v>
       </c>
       <c r="L37" s="0">
         <v>0</v>
@@ -4170,7 +4170,7 @@
         <v>208</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>694</v>
+        <v>673</v>
       </c>
       <c r="L38" s="0">
         <v>0</v>
@@ -4196,7 +4196,7 @@
         <v>289</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>696</v>
+        <v>728</v>
       </c>
       <c r="H39" t="s" s="0">
         <v>509</v>
@@ -4208,7 +4208,7 @@
         <v>164</v>
       </c>
       <c r="K39" t="s" s="0">
-        <v>695</v>
+        <v>727</v>
       </c>
       <c r="L39" s="0">
         <v>0</v>
@@ -4234,7 +4234,7 @@
         <v>290</v>
       </c>
       <c r="G40" t="s" s="0">
-        <v>698</v>
+        <v>730</v>
       </c>
       <c r="H40" t="s" s="0">
         <v>509</v>
@@ -4246,7 +4246,7 @@
         <v>165</v>
       </c>
       <c r="K40" t="s" s="0">
-        <v>697</v>
+        <v>729</v>
       </c>
       <c r="L40" s="0">
         <v>0</v>
@@ -4272,7 +4272,7 @@
         <v>290</v>
       </c>
       <c r="G41" t="s" s="0">
-        <v>700</v>
+        <v>732</v>
       </c>
       <c r="H41" t="s" s="0">
         <v>509</v>
@@ -4284,7 +4284,7 @@
         <v>166</v>
       </c>
       <c r="K41" t="s" s="0">
-        <v>699</v>
+        <v>731</v>
       </c>
       <c r="L41" s="0">
         <v>0</v>
@@ -4310,7 +4310,7 @@
         <v>290</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>702</v>
+        <v>734</v>
       </c>
       <c r="H42" t="s" s="0">
         <v>509</v>
@@ -4322,7 +4322,7 @@
         <v>167</v>
       </c>
       <c r="K42" t="s" s="0">
-        <v>701</v>
+        <v>733</v>
       </c>
       <c r="L42" s="0">
         <v>0</v>
@@ -4348,7 +4348,7 @@
         <v>291</v>
       </c>
       <c r="G43" t="s" s="0">
-        <v>704</v>
+        <v>736</v>
       </c>
       <c r="H43" t="s" s="0">
         <v>509</v>
@@ -4360,7 +4360,7 @@
         <v>168</v>
       </c>
       <c r="K43" t="s" s="0">
-        <v>703</v>
+        <v>735</v>
       </c>
       <c r="L43" s="0">
         <v>0</v>
@@ -4386,7 +4386,7 @@
         <v>292</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>706</v>
+        <v>738</v>
       </c>
       <c r="H44" t="s" s="0">
         <v>509</v>
@@ -4398,7 +4398,7 @@
         <v>169</v>
       </c>
       <c r="K44" t="s" s="0">
-        <v>705</v>
+        <v>737</v>
       </c>
       <c r="L44" s="0">
         <v>0</v>
@@ -4424,7 +4424,7 @@
         <v>293</v>
       </c>
       <c r="G45" t="s" s="0">
-        <v>708</v>
+        <v>740</v>
       </c>
       <c r="H45" t="s" s="0">
         <v>509</v>
@@ -4436,7 +4436,7 @@
         <v>170</v>
       </c>
       <c r="K45" t="s" s="0">
-        <v>707</v>
+        <v>739</v>
       </c>
       <c r="L45" s="0">
         <v>0</v>
@@ -4462,7 +4462,7 @@
         <v>294</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>710</v>
+        <v>742</v>
       </c>
       <c r="H46" t="s" s="0">
         <v>509</v>
@@ -4474,7 +4474,7 @@
         <v>171</v>
       </c>
       <c r="K46" t="s" s="0">
-        <v>709</v>
+        <v>741</v>
       </c>
       <c r="L46" s="0">
         <v>0</v>
@@ -4500,7 +4500,7 @@
         <v>295</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>712</v>
+        <v>744</v>
       </c>
       <c r="H47" t="s" s="0">
         <v>509</v>
@@ -4512,7 +4512,7 @@
         <v>172</v>
       </c>
       <c r="K47" t="s" s="0">
-        <v>711</v>
+        <v>743</v>
       </c>
       <c r="L47" s="0">
         <v>0</v>
@@ -4538,7 +4538,7 @@
         <v>280</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>714</v>
+        <v>746</v>
       </c>
       <c r="H48" t="s" s="0">
         <v>509</v>
@@ -4550,7 +4550,7 @@
         <v>155</v>
       </c>
       <c r="K48" t="s" s="0">
-        <v>713</v>
+        <v>745</v>
       </c>
       <c r="L48" s="0">
         <v>0</v>
@@ -4576,7 +4576,7 @@
         <v>296</v>
       </c>
       <c r="G49" t="s" s="0">
-        <v>716</v>
+        <v>748</v>
       </c>
       <c r="H49" t="s" s="0">
         <v>509</v>
@@ -4588,7 +4588,7 @@
         <v>173</v>
       </c>
       <c r="K49" t="s" s="0">
-        <v>715</v>
+        <v>747</v>
       </c>
       <c r="L49" s="0">
         <v>0</v>
@@ -4614,7 +4614,7 @@
         <v>287</v>
       </c>
       <c r="G50" t="s" s="0">
-        <v>718</v>
+        <v>750</v>
       </c>
       <c r="H50" t="s" s="0">
         <v>509</v>
@@ -4626,7 +4626,7 @@
         <v>174</v>
       </c>
       <c r="K50" t="s" s="0">
-        <v>717</v>
+        <v>749</v>
       </c>
       <c r="L50" s="0">
         <v>0</v>
@@ -4634,7 +4634,7 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>719</v>
+        <v>649</v>
       </c>
       <c r="B51" t="s" s="0">
         <v>87</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>720</v>
+        <v>650</v>
       </c>
       <c r="B52" t="s" s="0">
         <v>88</v>
@@ -4698,7 +4698,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>721</v>
+        <v>651</v>
       </c>
       <c r="B53" t="s" s="0">
         <v>541</v>
@@ -4730,7 +4730,7 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>722</v>
+        <v>652</v>
       </c>
       <c r="B54" t="s" s="0">
         <v>89</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>723</v>
+        <v>653</v>
       </c>
       <c r="B55" t="s" s="0">
         <v>86</v>
@@ -4836,7 +4836,7 @@
         <v>284</v>
       </c>
       <c r="G60" t="s" s="0">
-        <v>725</v>
+        <v>752</v>
       </c>
       <c r="H60" t="s" s="0">
         <v>509</v>
@@ -4848,7 +4848,7 @@
         <v>175</v>
       </c>
       <c r="K60" t="s" s="0">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="L60" s="0">
         <v>0</v>
@@ -4874,7 +4874,7 @@
         <v>299</v>
       </c>
       <c r="G61" t="s" s="0">
-        <v>727</v>
+        <v>754</v>
       </c>
       <c r="H61" t="s" s="0">
         <v>509</v>
@@ -4886,7 +4886,7 @@
         <v>176</v>
       </c>
       <c r="K61" t="s" s="0">
-        <v>726</v>
+        <v>753</v>
       </c>
       <c r="L61" s="0">
         <v>0</v>
@@ -4912,7 +4912,7 @@
         <v>284</v>
       </c>
       <c r="G62" t="s" s="0">
-        <v>729</v>
+        <v>756</v>
       </c>
       <c r="H62" t="s" s="0">
         <v>509</v>
@@ -4924,7 +4924,7 @@
         <v>177</v>
       </c>
       <c r="K62" t="s" s="0">
-        <v>728</v>
+        <v>755</v>
       </c>
       <c r="L62" s="0">
         <v>0</v>
@@ -4950,7 +4950,7 @@
         <v>277</v>
       </c>
       <c r="G63" t="s" s="0">
-        <v>731</v>
+        <v>758</v>
       </c>
       <c r="H63" t="s" s="0">
         <v>509</v>
@@ -4962,7 +4962,7 @@
         <v>178</v>
       </c>
       <c r="K63" t="s" s="0">
-        <v>730</v>
+        <v>757</v>
       </c>
       <c r="L63" s="0">
         <v>0</v>
@@ -4988,7 +4988,7 @@
         <v>297</v>
       </c>
       <c r="G64" t="s" s="0">
-        <v>733</v>
+        <v>760</v>
       </c>
       <c r="H64" t="s" s="0">
         <v>509</v>
@@ -5000,7 +5000,7 @@
         <v>179</v>
       </c>
       <c r="K64" t="s" s="0">
-        <v>732</v>
+        <v>759</v>
       </c>
       <c r="L64" s="0">
         <v>0</v>
@@ -5026,7 +5026,7 @@
         <v>286</v>
       </c>
       <c r="G65" t="s" s="0">
-        <v>735</v>
+        <v>762</v>
       </c>
       <c r="H65" t="s" s="0">
         <v>509</v>
@@ -5038,7 +5038,7 @@
         <v>180</v>
       </c>
       <c r="K65" t="s" s="0">
-        <v>734</v>
+        <v>761</v>
       </c>
       <c r="L65" s="0">
         <v>0</v>
@@ -5064,7 +5064,7 @@
         <v>284</v>
       </c>
       <c r="G66" t="s" s="0">
-        <v>737</v>
+        <v>764</v>
       </c>
       <c r="H66" t="s" s="0">
         <v>509</v>
@@ -5076,7 +5076,7 @@
         <v>181</v>
       </c>
       <c r="K66" t="s" s="0">
-        <v>736</v>
+        <v>763</v>
       </c>
       <c r="L66" s="0">
         <v>0</v>
@@ -5102,7 +5102,7 @@
         <v>280</v>
       </c>
       <c r="G67" t="s" s="0">
-        <v>739</v>
+        <v>766</v>
       </c>
       <c r="H67" t="s" s="0">
         <v>509</v>
@@ -5114,7 +5114,7 @@
         <v>182</v>
       </c>
       <c r="K67" t="s" s="0">
-        <v>738</v>
+        <v>765</v>
       </c>
       <c r="L67" s="0">
         <v>0</v>
@@ -5140,7 +5140,7 @@
         <v>277</v>
       </c>
       <c r="G68" t="s" s="0">
-        <v>741</v>
+        <v>768</v>
       </c>
       <c r="H68" t="s" s="0">
         <v>509</v>
@@ -5152,7 +5152,7 @@
         <v>183</v>
       </c>
       <c r="K68" t="s" s="0">
-        <v>740</v>
+        <v>767</v>
       </c>
       <c r="L68" s="0">
         <v>0</v>
@@ -5178,7 +5178,7 @@
         <v>300</v>
       </c>
       <c r="G69" t="s" s="0">
-        <v>743</v>
+        <v>770</v>
       </c>
       <c r="H69" t="s" s="0">
         <v>509</v>
@@ -5190,7 +5190,7 @@
         <v>184</v>
       </c>
       <c r="K69" t="s" s="0">
-        <v>742</v>
+        <v>769</v>
       </c>
       <c r="L69" s="0">
         <v>0</v>
@@ -5216,7 +5216,7 @@
         <v>297</v>
       </c>
       <c r="G70" t="s" s="0">
-        <v>745</v>
+        <v>772</v>
       </c>
       <c r="H70" t="s" s="0">
         <v>509</v>
@@ -5228,7 +5228,7 @@
         <v>185</v>
       </c>
       <c r="K70" t="s" s="0">
-        <v>744</v>
+        <v>771</v>
       </c>
       <c r="L70" s="0">
         <v>0</v>
@@ -5254,7 +5254,7 @@
         <v>284</v>
       </c>
       <c r="G71" t="s" s="0">
-        <v>746</v>
+        <v>773</v>
       </c>
       <c r="H71" t="s" s="0">
         <v>509</v>
@@ -5266,7 +5266,7 @@
         <v>175</v>
       </c>
       <c r="K71" t="s" s="0">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="L71" s="0">
         <v>0</v>
@@ -5292,7 +5292,7 @@
         <v>297</v>
       </c>
       <c r="G72" t="s" s="0">
-        <v>748</v>
+        <v>775</v>
       </c>
       <c r="H72" t="s" s="0">
         <v>509</v>
@@ -5304,7 +5304,7 @@
         <v>186</v>
       </c>
       <c r="K72" t="s" s="0">
-        <v>747</v>
+        <v>774</v>
       </c>
       <c r="L72" s="0">
         <v>0</v>
@@ -5330,7 +5330,7 @@
         <v>277</v>
       </c>
       <c r="G73" t="s" s="0">
-        <v>750</v>
+        <v>777</v>
       </c>
       <c r="H73" t="s" s="0">
         <v>509</v>
@@ -5342,7 +5342,7 @@
         <v>187</v>
       </c>
       <c r="K73" t="s" s="0">
-        <v>749</v>
+        <v>776</v>
       </c>
       <c r="L73" s="0">
         <v>0</v>
@@ -5368,7 +5368,7 @@
         <v>283</v>
       </c>
       <c r="G74" t="s" s="0">
-        <v>752</v>
+        <v>779</v>
       </c>
       <c r="H74" t="s" s="0">
         <v>509</v>
@@ -5380,7 +5380,7 @@
         <v>188</v>
       </c>
       <c r="K74" t="s" s="0">
-        <v>751</v>
+        <v>778</v>
       </c>
       <c r="L74" s="0">
         <v>0</v>
@@ -5406,7 +5406,7 @@
         <v>274</v>
       </c>
       <c r="G75" t="s" s="0">
-        <v>754</v>
+        <v>781</v>
       </c>
       <c r="H75" t="s" s="0">
         <v>509</v>
@@ -5418,7 +5418,7 @@
         <v>189</v>
       </c>
       <c r="K75" t="s" s="0">
-        <v>753</v>
+        <v>780</v>
       </c>
       <c r="L75" s="0">
         <v>0</v>
@@ -5444,7 +5444,7 @@
         <v>284</v>
       </c>
       <c r="G76" t="s" s="0">
-        <v>756</v>
+        <v>783</v>
       </c>
       <c r="H76" t="s" s="0">
         <v>509</v>
@@ -5456,7 +5456,7 @@
         <v>190</v>
       </c>
       <c r="K76" t="s" s="0">
-        <v>755</v>
+        <v>782</v>
       </c>
       <c r="L76" s="0">
         <v>0</v>
@@ -5482,7 +5482,7 @@
         <v>284</v>
       </c>
       <c r="G77" t="s" s="0">
-        <v>758</v>
+        <v>785</v>
       </c>
       <c r="H77" t="s" s="0">
         <v>509</v>
@@ -5494,7 +5494,7 @@
         <v>597</v>
       </c>
       <c r="K77" t="s" s="0">
-        <v>757</v>
+        <v>784</v>
       </c>
       <c r="L77" s="0">
         <v>0</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>759</v>
+        <v>654</v>
       </c>
       <c r="B79" t="s" s="0">
         <v>99</v>
@@ -5526,7 +5526,7 @@
         <v>280</v>
       </c>
       <c r="G79" t="s" s="0">
-        <v>762</v>
+        <v>787</v>
       </c>
       <c r="H79" t="s" s="0">
         <v>509</v>
@@ -5535,10 +5535,10 @@
         <v>208</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>760</v>
+        <v>674</v>
       </c>
       <c r="K79" t="s" s="0">
-        <v>761</v>
+        <v>786</v>
       </c>
       <c r="L79" s="0">
         <v>0</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>763</v>
+        <v>655</v>
       </c>
       <c r="B80" t="s" s="0">
         <v>541</v>
@@ -5564,7 +5564,7 @@
         <v>302</v>
       </c>
       <c r="G80" t="s" s="0">
-        <v>766</v>
+        <v>789</v>
       </c>
       <c r="H80" t="s" s="0">
         <v>509</v>
@@ -5573,10 +5573,10 @@
         <v>208</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>764</v>
+        <v>675</v>
       </c>
       <c r="K80" t="s" s="0">
-        <v>765</v>
+        <v>788</v>
       </c>
       <c r="L80" s="0">
         <v>0</v>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>767</v>
+        <v>656</v>
       </c>
       <c r="B81" t="s" s="0">
         <v>112</v>
@@ -5602,7 +5602,7 @@
         <v>280</v>
       </c>
       <c r="G81" t="s" s="0">
-        <v>770</v>
+        <v>791</v>
       </c>
       <c r="H81" t="s" s="0">
         <v>509</v>
@@ -5611,10 +5611,10 @@
         <v>213</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>768</v>
+        <v>676</v>
       </c>
       <c r="K81" t="s" s="0">
-        <v>769</v>
+        <v>790</v>
       </c>
       <c r="L81" s="0">
         <v>0</v>
@@ -5622,7 +5622,7 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>771</v>
+        <v>657</v>
       </c>
       <c r="B82" t="s" s="0">
         <v>100</v>
@@ -5640,7 +5640,7 @@
         <v>303</v>
       </c>
       <c r="G82" t="s" s="0">
-        <v>774</v>
+        <v>793</v>
       </c>
       <c r="H82" t="s" s="0">
         <v>509</v>
@@ -5649,10 +5649,10 @@
         <v>208</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>772</v>
+        <v>677</v>
       </c>
       <c r="K82" t="s" s="0">
-        <v>773</v>
+        <v>792</v>
       </c>
       <c r="L82" s="0">
         <v>0</v>
@@ -5660,7 +5660,7 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>775</v>
+        <v>658</v>
       </c>
       <c r="B83" t="s" s="0">
         <v>546</v>
@@ -5678,7 +5678,7 @@
         <v>297</v>
       </c>
       <c r="G83" t="s" s="0">
-        <v>778</v>
+        <v>795</v>
       </c>
       <c r="H83" t="s" s="0">
         <v>509</v>
@@ -5687,10 +5687,10 @@
         <v>221</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>776</v>
+        <v>678</v>
       </c>
       <c r="K83" t="s" s="0">
-        <v>777</v>
+        <v>794</v>
       </c>
       <c r="L83" s="0">
         <v>0</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>779</v>
+        <v>659</v>
       </c>
       <c r="B84" t="s" s="0">
         <v>541</v>
@@ -5716,7 +5716,7 @@
         <v>298</v>
       </c>
       <c r="G84" t="s" s="0">
-        <v>782</v>
+        <v>797</v>
       </c>
       <c r="H84" t="s" s="0">
         <v>509</v>
@@ -5725,10 +5725,10 @@
         <v>208</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>780</v>
+        <v>679</v>
       </c>
       <c r="K84" t="s" s="0">
-        <v>781</v>
+        <v>796</v>
       </c>
       <c r="L84" s="0">
         <v>0</v>
@@ -5760,7 +5760,7 @@
         <v>287</v>
       </c>
       <c r="G86" t="s" s="0">
-        <v>784</v>
+        <v>799</v>
       </c>
       <c r="H86" t="s" s="0">
         <v>509</v>
@@ -5772,7 +5772,7 @@
         <v>191</v>
       </c>
       <c r="K86" t="s" s="0">
-        <v>783</v>
+        <v>798</v>
       </c>
       <c r="L86" s="0">
         <v>0</v>
@@ -5798,7 +5798,7 @@
         <v>287</v>
       </c>
       <c r="G87" t="s" s="0">
-        <v>786</v>
+        <v>801</v>
       </c>
       <c r="H87" t="s" s="0">
         <v>509</v>
@@ -5810,7 +5810,7 @@
         <v>192</v>
       </c>
       <c r="K87" t="s" s="0">
-        <v>785</v>
+        <v>800</v>
       </c>
       <c r="L87" s="0">
         <v>0</v>
@@ -5836,7 +5836,7 @@
         <v>278</v>
       </c>
       <c r="G88" t="s" s="0">
-        <v>788</v>
+        <v>803</v>
       </c>
       <c r="H88" t="s" s="0">
         <v>509</v>
@@ -5848,7 +5848,7 @@
         <v>193</v>
       </c>
       <c r="K88" t="s" s="0">
-        <v>787</v>
+        <v>802</v>
       </c>
       <c r="L88" s="0">
         <v>0</v>
@@ -5874,7 +5874,7 @@
         <v>278</v>
       </c>
       <c r="G89" t="s" s="0">
-        <v>790</v>
+        <v>805</v>
       </c>
       <c r="H89" t="s" s="0">
         <v>509</v>
@@ -5886,7 +5886,7 @@
         <v>194</v>
       </c>
       <c r="K89" t="s" s="0">
-        <v>789</v>
+        <v>804</v>
       </c>
       <c r="L89" s="0">
         <v>0</v>
@@ -5912,7 +5912,7 @@
         <v>304</v>
       </c>
       <c r="G90" t="s" s="0">
-        <v>792</v>
+        <v>807</v>
       </c>
       <c r="H90" t="s" s="0">
         <v>509</v>
@@ -5924,7 +5924,7 @@
         <v>195</v>
       </c>
       <c r="K90" t="s" s="0">
-        <v>791</v>
+        <v>806</v>
       </c>
       <c r="L90" s="0">
         <v>0</v>
@@ -5950,7 +5950,7 @@
         <v>284</v>
       </c>
       <c r="G91" t="s" s="0">
-        <v>794</v>
+        <v>809</v>
       </c>
       <c r="H91" t="s" s="0">
         <v>509</v>
@@ -5962,7 +5962,7 @@
         <v>196</v>
       </c>
       <c r="K91" t="s" s="0">
-        <v>793</v>
+        <v>808</v>
       </c>
       <c r="L91" s="0">
         <v>0</v>
@@ -5988,7 +5988,7 @@
         <v>305</v>
       </c>
       <c r="G92" t="s" s="0">
-        <v>796</v>
+        <v>811</v>
       </c>
       <c r="H92" t="s" s="0">
         <v>509</v>
@@ -6000,7 +6000,7 @@
         <v>197</v>
       </c>
       <c r="K92" t="s" s="0">
-        <v>795</v>
+        <v>810</v>
       </c>
       <c r="L92" s="0">
         <v>0</v>
@@ -6026,7 +6026,7 @@
         <v>288</v>
       </c>
       <c r="G93" t="s" s="0">
-        <v>798</v>
+        <v>813</v>
       </c>
       <c r="H93" t="s" s="0">
         <v>509</v>
@@ -6038,7 +6038,7 @@
         <v>198</v>
       </c>
       <c r="K93" t="s" s="0">
-        <v>797</v>
+        <v>812</v>
       </c>
       <c r="L93" s="0">
         <v>0</v>
@@ -6064,7 +6064,7 @@
         <v>306</v>
       </c>
       <c r="G94" t="s" s="0">
-        <v>800</v>
+        <v>815</v>
       </c>
       <c r="H94" t="s" s="0">
         <v>509</v>
@@ -6076,7 +6076,7 @@
         <v>199</v>
       </c>
       <c r="K94" t="s" s="0">
-        <v>799</v>
+        <v>814</v>
       </c>
       <c r="L94" s="0">
         <v>0</v>
@@ -6102,7 +6102,7 @@
         <v>281</v>
       </c>
       <c r="G95" t="s" s="0">
-        <v>802</v>
+        <v>817</v>
       </c>
       <c r="H95" t="s" s="0">
         <v>509</v>
@@ -6114,7 +6114,7 @@
         <v>200</v>
       </c>
       <c r="K95" t="s" s="0">
-        <v>801</v>
+        <v>816</v>
       </c>
       <c r="L95" s="0">
         <v>0</v>
@@ -6175,7 +6175,7 @@
         <v>308</v>
       </c>
       <c r="G102" t="s" s="0">
-        <v>805</v>
+        <v>819</v>
       </c>
       <c r="H102" t="s" s="0">
         <v>509</v>
@@ -6184,10 +6184,10 @@
         <v>218</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>803</v>
+        <v>680</v>
       </c>
       <c r="K102" t="s" s="0">
-        <v>804</v>
+        <v>818</v>
       </c>
       <c r="L102" s="0">
         <v>0</v>
@@ -6213,7 +6213,7 @@
         <v>275</v>
       </c>
       <c r="G103" t="s" s="0">
-        <v>808</v>
+        <v>821</v>
       </c>
       <c r="H103" t="s" s="0">
         <v>509</v>
@@ -6222,10 +6222,10 @@
         <v>219</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>806</v>
+        <v>681</v>
       </c>
       <c r="K103" t="s" s="0">
-        <v>807</v>
+        <v>820</v>
       </c>
       <c r="L103" s="0">
         <v>0</v>
@@ -6251,7 +6251,7 @@
         <v>273</v>
       </c>
       <c r="G104" t="s" s="0">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="H104" t="s" s="0">
         <v>509</v>
@@ -6260,10 +6260,10 @@
         <v>225</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>809</v>
+        <v>682</v>
       </c>
       <c r="K104" t="s" s="0">
-        <v>810</v>
+        <v>822</v>
       </c>
       <c r="L104" s="0">
         <v>0</v>
@@ -6289,7 +6289,7 @@
         <v>297</v>
       </c>
       <c r="G105" t="s" s="0">
-        <v>814</v>
+        <v>825</v>
       </c>
       <c r="H105" t="s" s="0">
         <v>509</v>
@@ -6298,10 +6298,10 @@
         <v>208</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>812</v>
+        <v>683</v>
       </c>
       <c r="K105" t="s" s="0">
-        <v>813</v>
+        <v>824</v>
       </c>
       <c r="L105" s="0">
         <v>0</v>
@@ -6327,7 +6327,7 @@
         <v>297</v>
       </c>
       <c r="G106" t="s" s="0">
-        <v>817</v>
+        <v>827</v>
       </c>
       <c r="H106" t="s" s="0">
         <v>509</v>
@@ -6336,10 +6336,10 @@
         <v>226</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>815</v>
+        <v>684</v>
       </c>
       <c r="K106" t="s" s="0">
-        <v>816</v>
+        <v>826</v>
       </c>
       <c r="L106" s="0">
         <v>0</v>
@@ -6447,7 +6447,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>818</v>
+        <v>660</v>
       </c>
       <c r="B127" t="s" s="0">
         <v>96</v>
@@ -6465,7 +6465,7 @@
         <v>309</v>
       </c>
       <c r="G127" t="s" s="0">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="H127" t="s" s="0">
         <v>509</v>
@@ -6477,7 +6477,7 @@
         <v>603</v>
       </c>
       <c r="K127" t="s" s="0">
-        <v>819</v>
+        <v>828</v>
       </c>
       <c r="L127" s="0">
         <v>0</v>
@@ -6485,7 +6485,7 @@
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>821</v>
+        <v>661</v>
       </c>
       <c r="B128" t="s" s="0">
         <v>543</v>
@@ -6503,7 +6503,7 @@
         <v>310</v>
       </c>
       <c r="G128" t="s" s="0">
-        <v>823</v>
+        <v>831</v>
       </c>
       <c r="H128" t="s" s="0">
         <v>509</v>
@@ -6515,7 +6515,7 @@
         <v>598</v>
       </c>
       <c r="K128" t="s" s="0">
-        <v>822</v>
+        <v>830</v>
       </c>
       <c r="L128" s="0">
         <v>0</v>
@@ -6523,7 +6523,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>824</v>
+        <v>662</v>
       </c>
       <c r="B129" t="s" s="0">
         <v>97</v>
@@ -6541,7 +6541,7 @@
         <v>301</v>
       </c>
       <c r="G129" t="s" s="0">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="H129" t="s" s="0">
         <v>509</v>
@@ -6553,7 +6553,7 @@
         <v>201</v>
       </c>
       <c r="K129" t="s" s="0">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="L129" s="0">
         <v>0</v>
@@ -6561,7 +6561,7 @@
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>827</v>
+        <v>663</v>
       </c>
       <c r="B130" t="s" s="0">
         <v>68</v>
@@ -6579,7 +6579,7 @@
         <v>277</v>
       </c>
       <c r="G130" t="s" s="0">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="H130" t="s" s="0">
         <v>509</v>
@@ -6591,7 +6591,7 @@
         <v>202</v>
       </c>
       <c r="K130" t="s" s="0">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="L130" s="0">
         <v>0</v>
@@ -6599,7 +6599,7 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>830</v>
+        <v>664</v>
       </c>
       <c r="B131" t="s" s="0">
         <v>98</v>
@@ -6617,7 +6617,7 @@
         <v>307</v>
       </c>
       <c r="G131" t="s" s="0">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="H131" t="s" s="0">
         <v>509</v>
@@ -6629,7 +6629,7 @@
         <v>203</v>
       </c>
       <c r="K131" t="s" s="0">
-        <v>831</v>
+        <v>836</v>
       </c>
       <c r="L131" s="0">
         <v>0</v>
@@ -6637,7 +6637,7 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>833</v>
+        <v>665</v>
       </c>
       <c r="B132" t="s" s="0">
         <v>66</v>
@@ -6655,7 +6655,7 @@
         <v>307</v>
       </c>
       <c r="G132" t="s" s="0">
-        <v>835</v>
+        <v>839</v>
       </c>
       <c r="H132" t="s" s="0">
         <v>509</v>
@@ -6667,7 +6667,7 @@
         <v>204</v>
       </c>
       <c r="K132" t="s" s="0">
-        <v>834</v>
+        <v>838</v>
       </c>
       <c r="L132" s="0">
         <v>0</v>
@@ -6675,7 +6675,7 @@
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>836</v>
+        <v>666</v>
       </c>
       <c r="B133" t="s" s="0">
         <v>94</v>
@@ -6693,7 +6693,7 @@
         <v>305</v>
       </c>
       <c r="G133" t="s" s="0">
-        <v>838</v>
+        <v>841</v>
       </c>
       <c r="H133" t="s" s="0">
         <v>509</v>
@@ -6705,7 +6705,7 @@
         <v>604</v>
       </c>
       <c r="K133" t="s" s="0">
-        <v>837</v>
+        <v>840</v>
       </c>
       <c r="L133" s="0">
         <v>0</v>
@@ -6713,7 +6713,7 @@
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>839</v>
+        <v>667</v>
       </c>
       <c r="B134" t="s" s="0">
         <v>99</v>
@@ -6731,7 +6731,7 @@
         <v>311</v>
       </c>
       <c r="G134" t="s" s="0">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="H134" t="s" s="0">
         <v>509</v>
@@ -6743,7 +6743,7 @@
         <v>205</v>
       </c>
       <c r="K134" t="s" s="0">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="L134" s="0">
         <v>0</v>
@@ -6751,7 +6751,7 @@
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>842</v>
+        <v>668</v>
       </c>
       <c r="B135" t="s" s="0">
         <v>541</v>
@@ -6769,7 +6769,7 @@
         <v>301</v>
       </c>
       <c r="G135" t="s" s="0">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="H135" t="s" s="0">
         <v>509</v>
@@ -6781,7 +6781,7 @@
         <v>206</v>
       </c>
       <c r="K135" t="s" s="0">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="L135" s="0">
         <v>0</v>
@@ -6789,7 +6789,7 @@
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>845</v>
+        <v>669</v>
       </c>
       <c r="B136" t="s" s="0">
         <v>112</v>

</xml_diff>